<commit_message>
controller on entity delete + bug resolved
</commit_message>
<xml_diff>
--- a/data/solutre_hex_act.xlsx
+++ b/data/solutre_hex_act.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mregie01\SGE\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A80C081-0E5A-4709-89EA-32263AD04CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,7 +40,7 @@
     <t>vinBio</t>
   </si>
   <si>
-    <t>sou</t>
+    <t>sous</t>
   </si>
   <si>
     <t>touriste</t>
@@ -118,6 +112,9 @@
     <t>Vigne</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/V5_ACT.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">V6 </t>
   </si>
   <si>
@@ -187,364 +184,538 @@
     <t>Restauration des murets (V)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/V13_ACT.png</t>
+  </si>
+  <si>
     <t>N1</t>
   </si>
   <si>
     <t>Cycle de réunions publiques sur l'écologie</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N1_ACT.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">N2 </t>
   </si>
   <si>
     <t>Restauration des murets (N)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N2_ACT.png</t>
+  </si>
+  <si>
     <t>N3</t>
   </si>
   <si>
     <t>Restauration des murets (N2)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N3_ACT.png</t>
+  </si>
+  <si>
     <t>N4</t>
   </si>
   <si>
     <t>Demande de subventions</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N4_ACT.png</t>
+  </si>
+  <si>
     <t>N5</t>
   </si>
   <si>
     <t>Hébergement atypique : cabane</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N5_ACT.png</t>
+  </si>
+  <si>
     <t>N6</t>
   </si>
   <si>
     <t>Atlas de la biodiversité communale</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N6_ACT.png</t>
+  </si>
+  <si>
     <t>N7</t>
   </si>
   <si>
     <t>Garde-Champêtre</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N7_ACT.png</t>
+  </si>
+  <si>
     <t>N8</t>
   </si>
   <si>
     <t>Plan de relance du bocage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N8_ACT.png</t>
+  </si>
+  <si>
     <t>N9</t>
   </si>
   <si>
     <t>Certification forestière</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N9_ACT.png</t>
+  </si>
+  <si>
     <t>N10</t>
   </si>
   <si>
     <t>Sentier botanique</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N10_ACT.png</t>
+  </si>
+  <si>
     <t>N11</t>
   </si>
   <si>
     <t>Centre de soin de la faune sauvage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N11_ACT.png</t>
+  </si>
+  <si>
     <t>N12</t>
   </si>
   <si>
     <t xml:space="preserve">Zone d'interdiction de la chasse et de la pêche </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N12_ACT.png</t>
+  </si>
+  <si>
     <t>N13</t>
   </si>
   <si>
     <t>Camp de baguage d'oiseaux</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N13_ACT.png</t>
+  </si>
+  <si>
     <t>N14</t>
   </si>
   <si>
     <t>Guinguette bio éphémère</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N14_ACT.png</t>
+  </si>
+  <si>
     <t>N15</t>
   </si>
   <si>
     <t>Jardin partagé</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N15_ACT.png</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
     <t xml:space="preserve">Concours international d'œnologie </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E1_ACT.png</t>
+  </si>
+  <si>
     <t>E2</t>
   </si>
   <si>
     <t xml:space="preserve">Office du tourisme </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E2_ACT.png</t>
+  </si>
+  <si>
     <t>E3</t>
   </si>
   <si>
     <t xml:space="preserve">Rénovation des logements vacants </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E3_ACT.png</t>
+  </si>
+  <si>
     <t>E4</t>
   </si>
   <si>
     <t>Mise en place de conseils de villages</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E4_ACT.png</t>
+  </si>
+  <si>
     <t>E5</t>
   </si>
   <si>
     <t>Attribution de subventions</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E5_ACT.png</t>
+  </si>
+  <si>
     <t>E6</t>
   </si>
   <si>
     <t>Foire au vin BIO</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E6_ACT.png</t>
+  </si>
+  <si>
     <t>E7</t>
   </si>
   <si>
     <t>Création d'un Pôle d'Equilibre Territorial et Rural</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E7_ACT.png</t>
+  </si>
+  <si>
     <t>E8</t>
   </si>
   <si>
     <t>Rénovation des logements vacants 2</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E8_ACT.png</t>
+  </si>
+  <si>
     <t>E9</t>
   </si>
   <si>
     <t>Cabinet d'infirmiers</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E9_ACT.png</t>
+  </si>
+  <si>
     <t>E10</t>
   </si>
   <si>
     <t>Opération cœur de village</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E10_ACT.png</t>
+  </si>
+  <si>
     <t>E11</t>
   </si>
   <si>
     <t>Cumul de mandats</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E11_ACT.png</t>
+  </si>
+  <si>
     <t>E12</t>
   </si>
   <si>
     <t>Passage à faune (crapauduc)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E12_ACT.png</t>
+  </si>
+  <si>
     <t>E13</t>
   </si>
   <si>
     <t>Aire de camping-cars</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E13_ACT.png</t>
+  </si>
+  <si>
     <t>E14</t>
   </si>
   <si>
     <t>Arrêté Zéro Phyto</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E14_ACT.png</t>
+  </si>
+  <si>
     <t>E15</t>
   </si>
   <si>
     <t>Placette de compostage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E15_ACT.png</t>
+  </si>
+  <si>
     <t>H1</t>
   </si>
   <si>
     <t>Comité de soutien à la viticulture bio</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H1_ACT.png</t>
+  </si>
+  <si>
     <t>H2</t>
   </si>
   <si>
     <t>Chantier bénévole de débroussaillage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H2_ACT.png</t>
+  </si>
+  <si>
     <t>H3</t>
   </si>
   <si>
     <t>Inventaire des vignes : Biodivine</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H3_ACT.png</t>
+  </si>
+  <si>
     <t>H4</t>
   </si>
   <si>
     <t>Mouvement démocratique local</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H4_ACT.png</t>
+  </si>
+  <si>
     <t>H5</t>
   </si>
   <si>
     <t>Chambre d'hôtes</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H5_ACT.png</t>
+  </si>
+  <si>
     <t>H6</t>
   </si>
   <si>
     <t xml:space="preserve">Sensibilisation à la biodynamie au lycée agricole </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H6_ACT.png</t>
+  </si>
+  <si>
     <t>H7</t>
   </si>
   <si>
     <t>Lobbying associatif</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H7_ACT.png</t>
+  </si>
+  <si>
     <t>H8</t>
   </si>
   <si>
     <t xml:space="preserve">Salle de spectacles </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H8_ACT.png</t>
+  </si>
+  <si>
     <t>H9</t>
   </si>
   <si>
     <t>Association pour le label village étoilé</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H9_ACT.png</t>
+  </si>
+  <si>
     <t>H10</t>
   </si>
   <si>
     <t>EHPAD</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H10_ACT.png</t>
+  </si>
+  <si>
     <t>H11</t>
   </si>
   <si>
     <t>Salle des fêtes</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H11_ACT.png</t>
+  </si>
+  <si>
     <t>H12</t>
   </si>
   <si>
     <t>Bibliobus nature</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H12_ACT.png</t>
+  </si>
+  <si>
     <t>H13</t>
   </si>
   <si>
     <t>Refuge Ligue Protection des oiseaux</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H13_ACT.png</t>
+  </si>
+  <si>
     <t>H14</t>
   </si>
   <si>
     <t>Éco-pâturage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H14_ACT.png</t>
+  </si>
+  <si>
     <t>H15</t>
   </si>
   <si>
     <t>Festival de musique</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H15_ACT.png</t>
+  </si>
+  <si>
     <t>T1</t>
   </si>
   <si>
     <t>Restaurant gastronomique</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T1_ACT.png</t>
+  </si>
+  <si>
     <t>T2</t>
   </si>
   <si>
     <t>Aérodrome/héliport</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T2_ACT.png</t>
+  </si>
+  <si>
     <t>T3</t>
   </si>
   <si>
     <t>Marché nocturne</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T3_ACT.png</t>
+  </si>
+  <si>
     <t>T4</t>
   </si>
   <si>
     <t>Mission locale</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T4_ACT.png</t>
+  </si>
+  <si>
     <t>T5</t>
   </si>
   <si>
     <t>Hôtel</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T5_ACT.png</t>
+  </si>
+  <si>
     <t>T6</t>
   </si>
   <si>
     <t xml:space="preserve">Hall de dégustation </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T6_ACT.png</t>
+  </si>
+  <si>
     <t>T7</t>
   </si>
   <si>
     <t>Hôtel de luxe</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T7_ACT.png</t>
+  </si>
+  <si>
     <t>T8</t>
   </si>
   <si>
     <t>Cycle de conférences sur l'écologie</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T8_ACT.png</t>
+  </si>
+  <si>
     <t>T9</t>
   </si>
   <si>
     <t>Parking Camping-Car</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T9_ACT.png</t>
+  </si>
+  <si>
     <t>T10</t>
   </si>
   <si>
     <t>Bar d'hôtel</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T10_ACT.png</t>
+  </si>
+  <si>
     <t>T11</t>
   </si>
   <si>
     <t>Brasserie</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T11_ACT.png</t>
+  </si>
+  <si>
     <t>T12</t>
   </si>
   <si>
     <t>Épicerie fine</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T12_ACT.png</t>
+  </si>
+  <si>
     <t>T13</t>
   </si>
   <si>
     <t>Woofing</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T13_ACT.png</t>
+  </si>
+  <si>
     <t>T14</t>
   </si>
   <si>
-    <t xml:space="preserve">P1	Chambre d'hôtes du plateau	Plateau	[Plateau]
-P2	Vigne du plateau	Plateau	[Plateau]
-P3	Caveau du plateau	Plateau	[Plateau]
-P1	Chambre d'hôtes du plateau	Plateau	[Plateau]
-P2	Vigne du plateau	Plateau	[Plateau]
-P3	Caveau du plateau	Plateau	[Plateau]
-</t>
+    <t>./icon/solutre/hex/T14_ACT.png</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
   <si>
     <t>Chambre d'hôtes du plateau</t>
@@ -575,196 +746,14 @@
   </si>
   <si>
     <t>Observatoire ornithologique</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/V5_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/V13_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N1_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N2_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N3_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N4_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N5_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N6_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N7_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N8_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N9_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N10_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N11_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N12_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N13_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N14_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N15_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E1_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E2_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E3_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E4_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E5_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E6_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E7_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E8_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E9_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E10_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E11_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E12_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E13_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E14_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E15_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T1_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T2_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T3_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T4_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T5_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T6_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T7_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T8_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T9_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T10_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T11_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T12_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T13_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T14_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H1_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H2_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H3_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H4_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H5_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H6_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H7_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H8_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H9_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H10_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H11_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H12_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H13_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H14_ACT.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H15_ACT.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,12 +764,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -812,43 +795,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -859,10 +840,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -900,71 +881,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -992,7 +973,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1015,11 +996,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1028,13 +1009,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1044,7 +1025,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1053,7 +1034,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1062,7 +1043,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1070,10 +1051,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1138,31 +1119,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="4.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="49.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="8" width="27.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1296,7 +1285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1326,7 +1315,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1353,15 +1342,15 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1383,15 +1372,15 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1409,15 +1398,15 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1435,15 +1424,15 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1461,15 +1450,15 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1493,15 +1482,15 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -1525,15 +1514,15 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1551,15 +1540,15 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1582,16 +1571,16 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R14" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1609,15 +1598,15 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1635,15 +1624,15 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
@@ -1665,15 +1654,15 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -1695,15 +1684,15 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1725,15 +1714,15 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1751,15 +1740,15 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1777,15 +1766,15 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
@@ -1807,15 +1796,15 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1833,15 +1822,15 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1859,15 +1848,15 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -1891,15 +1880,15 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1917,15 +1906,15 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -1947,15 +1936,15 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -1979,15 +1968,15 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C29" s="3">
         <v>2</v>
@@ -2009,15 +1998,15 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2035,15 +2024,15 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2064,16 +2053,16 @@
         <v>1</v>
       </c>
       <c r="Q31" s="3"/>
-      <c r="R31" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R31" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2093,15 +2082,15 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2119,15 +2108,15 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2145,15 +2134,15 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2171,15 +2160,15 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2197,15 +2186,15 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2225,15 +2214,15 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2251,15 +2240,15 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2277,15 +2266,15 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -2303,15 +2292,15 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
@@ -2333,15 +2322,15 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -2363,15 +2352,15 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -2393,15 +2382,15 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2419,15 +2408,15 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -2449,15 +2438,15 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -2475,15 +2464,15 @@
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
@@ -2505,15 +2494,15 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -2531,15 +2520,15 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2561,15 +2550,15 @@
         <v>1</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -2593,15 +2582,15 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2619,15 +2608,15 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2645,15 +2634,15 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -2671,15 +2660,15 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2697,15 +2686,15 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2723,15 +2712,15 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2749,15 +2738,15 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="C57" s="3">
         <v>1</v>
@@ -2779,15 +2768,15 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2805,15 +2794,15 @@
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="C59" s="3">
         <v>1</v>
@@ -2835,15 +2824,15 @@
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
       <c r="R59" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2861,15 +2850,15 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
       <c r="R60" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>148</v>
+        <v>196</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2887,15 +2876,15 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
       <c r="R61" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2912,16 +2901,16 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
-      <c r="R62" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R62" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>152</v>
+        <v>202</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -2939,15 +2928,15 @@
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2969,15 +2958,15 @@
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2995,15 +2984,15 @@
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
       <c r="R65" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -3025,15 +3014,15 @@
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -3051,15 +3040,15 @@
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
       <c r="R67" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="C68" s="3">
         <v>1</v>
@@ -3081,15 +3070,15 @@
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="1" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="C69" s="3">
         <v>1</v>
@@ -3111,15 +3100,15 @@
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
       <c r="R69" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="1" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
@@ -3141,15 +3130,15 @@
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+      <c r="A71" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="B71" s="1" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="C71" s="3">
         <v>1</v>
@@ -3173,15 +3162,15 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="1" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
@@ -3203,15 +3192,15 @@
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
       <c r="R72" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="1" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -3231,101 +3220,107 @@
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
       <c r="R73" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="5" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6">
-        <v>1</v>
-      </c>
-      <c r="O74" s="6">
-        <v>1</v>
-      </c>
-      <c r="P74" s="6"/>
-      <c r="Q74" s="6"/>
+        <v>234</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3">
+        <v>1</v>
+      </c>
+      <c r="O74" s="3">
+        <v>1</v>
+      </c>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
       <c r="R74" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="5" t="s">
-        <v>175</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+      <c r="A75" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C75" s="6">
-        <v>1</v>
-      </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-      <c r="Q75" s="6"/>
+        <v>237</v>
+      </c>
+      <c r="C75" s="3">
+        <v>1</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3">
+        <v>1</v>
+      </c>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
       <c r="R75" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
-        <v>178</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+      <c r="A76" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C76" s="6">
-        <v>1</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-      <c r="Q76" s="6"/>
+        <v>240</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1</v>
+      </c>
+      <c r="D76" s="3">
+        <v>1</v>
+      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3">
+        <v>1</v>
+      </c>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
       <c r="R76" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="1" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>

</xml_diff>

<commit_message>
nettoyage de Solutre terminé. Reste le bug des conditions non prises en compte
</commit_message>
<xml_diff>
--- a/data/solutre_hex_act.xlsx
+++ b/data/solutre_hex_act.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbecu\Modelling\SGE\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22D7FF0-4B2E-4809-BF6A-296149C2F351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="242">
   <si>
     <t>id</t>
   </si>
@@ -740,19 +746,12 @@
   </si>
   <si>
     <t>./icon/solutre/hex/P3.png</t>
-  </si>
-  <si>
-    <t>T15</t>
-  </si>
-  <si>
-    <t>Observatoire ornithologique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -796,40 +795,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -840,10 +838,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -881,71 +879,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -973,7 +971,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -996,11 +994,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1009,13 +1007,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1025,7 +1023,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1034,7 +1032,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1043,7 +1041,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1051,10 +1049,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1119,39 +1117,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="4.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="49.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="7" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="27.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="4.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.44140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1233,7 +1223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1259,7 +1249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1285,7 +1275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1315,7 +1305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1345,7 +1335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1375,7 +1365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1401,7 +1391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1427,7 +1417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1453,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1485,7 +1475,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -1517,7 +1507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1543,7 +1533,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1575,7 +1565,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1601,7 +1591,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1627,7 +1617,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1657,7 +1647,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1687,7 +1677,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
@@ -1717,7 +1707,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1743,7 +1733,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
@@ -1769,7 +1759,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -1799,7 +1789,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -1825,7 +1815,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
@@ -1851,7 +1841,7 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -1883,7 +1873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -1909,7 +1899,7 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>93</v>
       </c>
@@ -1939,7 +1929,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>96</v>
       </c>
@@ -1971,7 +1961,7 @@
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>99</v>
       </c>
@@ -2001,7 +1991,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
@@ -2027,7 +2017,7 @@
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>105</v>
       </c>
@@ -2057,7 +2047,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>108</v>
       </c>
@@ -2085,7 +2075,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>111</v>
       </c>
@@ -2111,7 +2101,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
@@ -2137,7 +2127,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>117</v>
       </c>
@@ -2163,7 +2153,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>120</v>
       </c>
@@ -2189,7 +2179,7 @@
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>123</v>
       </c>
@@ -2217,7 +2207,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>126</v>
       </c>
@@ -2243,7 +2233,7 @@
         <v>128</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
@@ -2269,7 +2259,7 @@
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>132</v>
       </c>
@@ -2295,7 +2285,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>135</v>
       </c>
@@ -2325,7 +2315,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row r="42" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>138</v>
       </c>
@@ -2355,7 +2345,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row r="43" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>141</v>
       </c>
@@ -2385,7 +2375,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row r="44" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>144</v>
       </c>
@@ -2411,7 +2401,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row r="45" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>147</v>
       </c>
@@ -2441,7 +2431,7 @@
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row r="46" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>150</v>
       </c>
@@ -2467,7 +2457,7 @@
         <v>152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row r="47" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>153</v>
       </c>
@@ -2497,7 +2487,7 @@
         <v>155</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row r="48" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>156</v>
       </c>
@@ -2523,7 +2513,7 @@
         <v>158</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row r="49" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>159</v>
       </c>
@@ -2553,7 +2543,7 @@
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row r="50" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>162</v>
       </c>
@@ -2585,7 +2575,7 @@
         <v>164</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row r="51" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>165</v>
       </c>
@@ -2611,7 +2601,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row r="52" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
@@ -2637,7 +2627,7 @@
         <v>170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row r="53" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
@@ -2663,7 +2653,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row r="54" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>174</v>
       </c>
@@ -2689,7 +2679,7 @@
         <v>176</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row r="55" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>177</v>
       </c>
@@ -2715,7 +2705,7 @@
         <v>179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row r="56" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>180</v>
       </c>
@@ -2741,7 +2731,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row r="57" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>183</v>
       </c>
@@ -2771,7 +2761,7 @@
         <v>185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row r="58" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>186</v>
       </c>
@@ -2797,7 +2787,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row r="59" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>189</v>
       </c>
@@ -2827,7 +2817,7 @@
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row r="60" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>192</v>
       </c>
@@ -2853,7 +2843,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row r="61" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>195</v>
       </c>
@@ -2879,7 +2869,7 @@
         <v>197</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row r="62" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>198</v>
       </c>
@@ -2905,7 +2895,7 @@
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row r="63" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>201</v>
       </c>
@@ -2931,7 +2921,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row r="64" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>204</v>
       </c>
@@ -2961,7 +2951,7 @@
         <v>206</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row r="65" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>207</v>
       </c>
@@ -2987,7 +2977,7 @@
         <v>209</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+    <row r="66" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>210</v>
       </c>
@@ -3017,7 +3007,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+    <row r="67" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>213</v>
       </c>
@@ -3043,7 +3033,7 @@
         <v>215</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+    <row r="68" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>216</v>
       </c>
@@ -3073,7 +3063,7 @@
         <v>218</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+    <row r="69" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>219</v>
       </c>
@@ -3103,7 +3093,7 @@
         <v>221</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+    <row r="70" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>222</v>
       </c>
@@ -3133,7 +3123,7 @@
         <v>224</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+    <row r="71" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>225</v>
       </c>
@@ -3165,7 +3155,7 @@
         <v>227</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+    <row r="72" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>228</v>
       </c>
@@ -3195,7 +3185,7 @@
         <v>230</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+    <row r="73" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>231</v>
       </c>
@@ -3223,7 +3213,7 @@
         <v>232</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+    <row r="74" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>233</v>
       </c>
@@ -3253,7 +3243,7 @@
         <v>235</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row r="75" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>236</v>
       </c>
@@ -3283,7 +3273,7 @@
         <v>238</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row r="76" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>239</v>
       </c>
@@ -3315,30 +3305,6 @@
         <v>241</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
-      <c r="A77" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>